<commit_message>
added latlng to dataset
</commit_message>
<xml_diff>
--- a/datasets/full_analysis/handwritten_latlng.xlsx
+++ b/datasets/full_analysis/handwritten_latlng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kaede\Documents\GitHub\BIOL417_CORAL\datasets\full_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507B3572-25BE-4D14-8E4F-9C5D539EC009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3A74B9-75D3-4967-9664-386585CDBB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="0" windowWidth="16245" windowHeight="15150" xr2:uid="{6DDFC618-C846-4719-91AB-232509781086}"/>
+    <workbookView xWindow="0" yWindow="1770" windowWidth="14640" windowHeight="13380" xr2:uid="{6DDFC618-C846-4719-91AB-232509781086}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="156">
   <si>
     <t>doi</t>
   </si>
@@ -296,9 +296,6 @@
   </si>
   <si>
     <t>Column1</t>
-  </si>
-  <si>
-    <t>43°41'10''N, 7°19'0''E</t>
   </si>
   <si>
     <t>10.1155/2012/746720</t>
@@ -318,21 +315,6 @@
 Portofino, Italy (44°18'N 9°12'E)</t>
   </si>
   <si>
-    <t>48°42'48.17''N, 3°54'04.28''W</t>
-  </si>
-  <si>
-    <t>22°40'N, 121°27'E</t>
-  </si>
-  <si>
-    <t>22°40'N, 121°28'E</t>
-  </si>
-  <si>
-    <t>24°56.080''N, 81°50.143''W</t>
-  </si>
-  <si>
-    <t>41°50'N, 8°45'E</t>
-  </si>
-  <si>
     <t>35°03'51.8"N, 138°49'04.8"E</t>
   </si>
   <si>
@@ -348,9 +330,6 @@
     <t>28°47'52.9"N, 48°18'59.4"E</t>
   </si>
   <si>
-    <t>22°18'19.98″N, 38°57'46.08″E</t>
-  </si>
-  <si>
     <t>Orpheus Island Great Barrier Reef</t>
   </si>
   <si>
@@ -378,21 +357,6 @@
     <t>Al-Fahal reef</t>
   </si>
   <si>
-    <t>26°18.068''N, 80°04.112''W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25°31.478''N, 79°17.948''W </t>
-  </si>
-  <si>
-    <t>18°36.878''S, 146°29.990'E</t>
-  </si>
-  <si>
-    <t>5°36.8150''N, 103°03.418''E</t>
-  </si>
-  <si>
-    <t>37°04'09.6''N, 8°19'52.1''W</t>
-  </si>
-  <si>
     <t>Bimini, Tuna Alley</t>
   </si>
   <si>
@@ -420,9 +384,6 @@
     <t>NR_169415.1</t>
   </si>
   <si>
-    <t>21°56.9′N, 120°48.5′E</t>
-  </si>
-  <si>
     <t>10.1099/ijsem.0.002194</t>
   </si>
   <si>
@@ -432,9 +393,6 @@
     <t>Endozoicomonas sp. Acr-14</t>
   </si>
   <si>
-    <t>22°15.100’N, 38°57.386’E</t>
-  </si>
-  <si>
     <t>Red Sea</t>
   </si>
   <si>
@@ -447,9 +405,6 @@
     <t>Kenting</t>
   </si>
   <si>
-    <t>21˚56'20.2''N, 120˚44'44.6''E</t>
-  </si>
-  <si>
     <t>Florida Keys, Florida</t>
   </si>
   <si>
@@ -474,15 +429,6 @@
     <t>Okinawa</t>
   </si>
   <si>
-    <t>26˚37'42.2''N, 127˚51'35.6''E</t>
-  </si>
-  <si>
-    <t>25°11.9''N, 80°30.2''W</t>
-  </si>
-  <si>
-    <t>20°48.399'N, 156° 36.064'W</t>
-  </si>
-  <si>
     <t>OL957501</t>
   </si>
   <si>
@@ -505,6 +451,69 @@
   </si>
   <si>
     <t>OL957500</t>
+  </si>
+  <si>
+    <t>20°48'39.9"N, 156°36'06.4"W</t>
+  </si>
+  <si>
+    <t>37°04'09.6"N, 8°19'52.1"W</t>
+  </si>
+  <si>
+    <t>22°40"N, 121°27"E</t>
+  </si>
+  <si>
+    <t>22°40"N, 121°28"E</t>
+  </si>
+  <si>
+    <t>21°56'9"N, 120°48'5"E</t>
+  </si>
+  <si>
+    <t>43°41'10"N, 7°19'0"E</t>
+  </si>
+  <si>
+    <t>48°42'48.17"N, 3°54'04.28"W</t>
+  </si>
+  <si>
+    <t>41°50"N, 8°45"E</t>
+  </si>
+  <si>
+    <t>21°52'35"N, 120°43'29"E</t>
+  </si>
+  <si>
+    <t>22°18'19.98"N, 38°57'46.08"E</t>
+  </si>
+  <si>
+    <t>21˚56'20.2"N, 120˚44'44.6"E</t>
+  </si>
+  <si>
+    <t>26˚37'42.2"N, 127˚51'35.6"E</t>
+  </si>
+  <si>
+    <t>25°11.9"N, 80°30.2"W</t>
+  </si>
+  <si>
+    <t>22°15'10.0"N, 38°57'38.6"E</t>
+  </si>
+  <si>
+    <t>22°15.100"N, 38°57'38.6"E</t>
+  </si>
+  <si>
+    <t>5°36.8150"N, 103°03'41.8"E</t>
+  </si>
+  <si>
+    <t>18°36'87.8"S, 146°29'99.0"E</t>
+  </si>
+  <si>
+    <t>24°56'08.0"N, 81°50'14.3"W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25°31'47.8"N, 79°17'94.8"W </t>
+  </si>
+  <si>
+    <t>26°18'06.8"N, 80°04'11.2"W</t>
+  </si>
+  <si>
+    <t>10.1128/mSystems.01249-20</t>
   </si>
 </sst>
 </file>
@@ -652,7 +661,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -663,10 +672,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -679,9 +685,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -692,25 +697,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="15" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -721,28 +722,6 @@
     <cellStyle name="Normal 3" xfId="2" xr:uid="{C05CEA0E-E959-491D-92E1-8F888B870670}"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -851,6 +830,28 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -865,21 +866,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B606DC5D-4B20-4EF6-B9EF-8C66D03C7BCD}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B606DC5D-4B20-4EF6-B9EF-8C66D03C7BCD}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I30" xr:uid="{B606DC5D-4B20-4EF6-B9EF-8C66D03C7BCD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I30">
     <sortCondition ref="B1:B30"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9C193BD4-5343-437F-8A49-6FD1C559D51D}" name="doi" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{F0F03908-3F9B-42F4-87EF-551066C51895}" name="group" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{C350C942-3AFF-49F4-BE4D-5F28A120903B}" name="country" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{E69288E2-B5ED-46A0-A2F5-F9CF7D91999E}" name="source" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{224FF763-763D-4249-9E4B-94A91587474F}" name="latlng" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D8BDCAE8-3881-4D7B-A6BF-8E10B3D96A47}" name="date" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D2901B74-5DCE-46F7-B834-2C1B1C7CA5BC}" name="Column1" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{38C886A5-7B3A-471E-B260-8A3A6A06BC23}" name="notes" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{56377235-B5B6-417C-9348-40C4CBDD966F}" name="citation" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9C193BD4-5343-437F-8A49-6FD1C559D51D}" name="doi" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{F0F03908-3F9B-42F4-87EF-551066C51895}" name="group" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{C350C942-3AFF-49F4-BE4D-5F28A120903B}" name="country" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E69288E2-B5ED-46A0-A2F5-F9CF7D91999E}" name="source" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{224FF763-763D-4249-9E4B-94A91587474F}" name="latlng" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{D8BDCAE8-3881-4D7B-A6BF-8E10B3D96A47}" name="date" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{D2901B74-5DCE-46F7-B834-2C1B1C7CA5BC}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{38C886A5-7B3A-471E-B260-8A3A6A06BC23}" name="notes" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{56377235-B5B6-417C-9348-40C4CBDD966F}" name="citation" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1185,90 +1186,89 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="9" customWidth="1"/>
-    <col min="2" max="3" width="15.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="33" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" style="9" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="16" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="9" t="s">
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="9" t="s">
-        <v>116</v>
+      <c r="D2" t="s">
+        <v>104</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F2" s="7">
         <v>37043</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="9" t="s">
-        <v>116</v>
+      <c r="D3" t="s">
+        <v>104</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F3" s="7">
         <v>37043</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1281,136 +1281,134 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="28">
+        <v>90</v>
+      </c>
+      <c r="F4" s="23">
         <v>40026</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22" t="s">
+      <c r="D5" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="E5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="7">
         <v>39904</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" t="s">
         <v>81</v>
       </c>
-      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" s="30">
+      <c r="D6" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="25">
         <v>40345</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" s="31">
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="1">
         <v>39630</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="31">
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="1">
         <v>41730</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="32">
+      <c r="E9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="26">
         <v>41837</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="34">
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="1">
         <v>39234</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -1418,355 +1416,355 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="9" t="s">
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="1">
+        <v>39479</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12" s="1">
+        <v>40330</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="1">
+        <v>39783</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="1">
+        <v>39783</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="1">
+        <v>39965</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="31">
-        <v>39479</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="31">
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="1">
+        <v>39995</v>
+      </c>
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="27">
         <v>40330</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="31">
-        <v>39783</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="31">
-        <v>39783</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" s="31">
-        <v>39965</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F16" s="31">
-        <v>39995</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="B17" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="35">
-        <v>40330</v>
-      </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="31">
+      <c r="D18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" s="1">
         <v>40299</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>149</v>
+      <c r="C19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>131</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="31">
+        <v>142</v>
+      </c>
+      <c r="F19" s="1">
         <v>41365</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>89</v>
+      <c r="H19" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="30">
+      <c r="A20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" s="25">
         <v>42186</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F21" s="30">
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" s="25">
         <v>42186</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="H21" s="36"/>
+      <c r="G21" t="s">
+        <v>113</v>
+      </c>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="31">
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22" s="1">
         <v>41944</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="31" t="s">
+      <c r="H22" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="B23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F23" s="1">
+        <v>41183</v>
+      </c>
+      <c r="H23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="25">
+        <v>43235</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="B23" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="31">
-        <v>41183</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="9" t="s">
+    <row r="25" spans="1:9">
+      <c r="A25" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F25" s="25">
+        <v>43235</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="F24" s="30">
-        <v>43235</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="F25" s="30">
-        <v>43235</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" s="31">
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="1">
         <v>42979</v>
       </c>
       <c r="G26" s="2" t="s">
@@ -1774,20 +1772,20 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="31">
+      <c r="A27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="1">
         <v>43009</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -1795,20 +1793,20 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="F28" s="31">
+      <c r="A28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" t="s">
+        <v>145</v>
+      </c>
+      <c r="F28" s="1">
         <v>42979</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -1816,20 +1814,20 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="25" t="s">
+      <c r="A29" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="21"/>
+      <c r="D29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="F29" s="31">
+      <c r="F29" s="1">
         <v>42979</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -1837,32 +1835,35 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F30" s="34">
+      <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" s="1">
         <v>43739</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" spans="1:9">
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
+      <c r="A32" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1890,11 +1891,14 @@
     <hyperlink ref="A26" r:id="rId21" display="https://doi.org/10.1126/sciadv.abo2431" xr:uid="{820BA790-75F6-4ECE-956B-ED7A16802F0E}"/>
     <hyperlink ref="A29" r:id="rId22" display="https://doi.org/10.1126/sciadv.abo2431" xr:uid="{7D019800-0443-40E4-BC27-CDF61C3AE2DF}"/>
     <hyperlink ref="A28" r:id="rId23" display="https://doi.org/10.1126/sciadv.abo2431" xr:uid="{01648AE3-89C3-497E-BF81-FE3FA10BB19D}"/>
+    <hyperlink ref="A24" r:id="rId24" xr:uid="{AB645030-0C12-4D33-97A1-0AB32FD650B7}"/>
+    <hyperlink ref="A25" r:id="rId25" xr:uid="{C41D45F6-DDBD-4E71-9CB1-0A41FBFD51A5}"/>
+    <hyperlink ref="A32" r:id="rId26" xr:uid="{C51E5EC4-E578-4F5D-BF84-1C16392CE360}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
   <tableParts count="1">
-    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId28"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1904,7 +1908,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2076,49 +2080,49 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.5">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="D9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="13">
         <v>40026</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:7" ht="16.5">
-      <c r="A10" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>122</v>
+      <c r="A10" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="18">
+        <v>91</v>
+      </c>
+      <c r="E10" s="15">
         <v>42186</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:7" ht="16.5">
-      <c r="A11" s="19"/>
-      <c r="B11" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="2"/>
     </row>
   </sheetData>

</xml_diff>